<commit_message>
preenchendo coluna em branco
</commit_message>
<xml_diff>
--- a/01_raw_data/teste_segundo_grafico_fechado.xlsx
+++ b/01_raw_data/teste_segundo_grafico_fechado.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://klabin-my.sharepoint.com/personal/flavia_lemos_klabin_com_br/Documents/Documentos/14. Projeto de Estágio - report Woodstock/03. Análises Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://klabin-my.sharepoint.com/personal/flavia_lemos_klabin_com_br/Documents/Documentos/14. Projeto de Estágio - report Woodstock/04. Projetos/20240930_testes_ggplot_plotly_echarts/01_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_7FFB8877997DE9C425C8A68750BAE224592FC65C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{441A90A0-8B87-456B-B20E-F5284EF060C6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6420"/>
+    <workbookView xWindow="20370" yWindow="-2190" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Estoque de Euc Processo - 6 anos</t>
   </si>
@@ -34,11 +35,14 @@
   <si>
     <t>Estoque de Euc Processo - 8_100 anos</t>
   </si>
+  <si>
+    <t>classe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,11 +354,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,6 +373,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1">
         <v>2020</v>
       </c>
@@ -631,6 +638,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e28b46ea-2dae-4fb2-a087-8e68b2da7864" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010034F734616D3A2440B52E8BDC9FB6894E" ma:contentTypeVersion="15" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="a2e0d1567c0d8dce92c77b1015e46e3f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e28b46ea-2dae-4fb2-a087-8e68b2da7864" xmlns:ns4="b289068e-3945-41a1-bc46-895d4b4afa93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1c39c3e3b3210c9dabca3e2153f4a1fd" ns3:_="" ns4:_="">
     <xsd:import namespace="e28b46ea-2dae-4fb2-a087-8e68b2da7864"/>
@@ -863,24 +887,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2392F6D6-1E87-4054-8869-DC103E31DF0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e28b46ea-2dae-4fb2-a087-8e68b2da7864"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b289068e-3945-41a1-bc46-895d4b4afa93"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e28b46ea-2dae-4fb2-a087-8e68b2da7864" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4A7E5FE-23AC-464E-9810-CE8718CF2B7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A0C03D9-250F-435A-B802-403C11CB7C5D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -897,29 +929,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4A7E5FE-23AC-464E-9810-CE8718CF2B7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2392F6D6-1E87-4054-8869-DC103E31DF0A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e28b46ea-2dae-4fb2-a087-8e68b2da7864"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b289068e-3945-41a1-bc46-895d4b4afa93"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>